<commit_message>
dia 5 clases lista
</commit_message>
<xml_diff>
--- a/CSHARP1.xlsx
+++ b/CSHARP1.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ejemplos codigo" sheetId="3" r:id="rId1"/>
     <sheet name="instalar visual studio" sheetId="4" r:id="rId2"/>
     <sheet name="metodovacio" sheetId="5" r:id="rId3"/>
     <sheet name="metododevuelve" sheetId="6" r:id="rId4"/>
-    <sheet name="Hoja1" sheetId="8" r:id="rId5"/>
+    <sheet name="calculadora" sheetId="8" r:id="rId5"/>
     <sheet name="lenguaje tecnico" sheetId="7" r:id="rId6"/>
+    <sheet name="instanciar clases" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="184">
   <si>
     <t>Este programa calcula la suma de tres números y muestra el resultado por consola.</t>
   </si>
@@ -1212,13 +1213,162 @@
   </si>
   <si>
     <t>30/</t>
+  </si>
+  <si>
+    <t>MessageBox.Show("hola darwin");</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cedula</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {  get; set; }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public void </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Saludo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(){</t>
+    </r>
+  </si>
+  <si>
+    <t>asignar valor</t>
+  </si>
+  <si>
+    <t>tipo de dato</t>
+  </si>
+  <si>
+    <t>nombre variable</t>
+  </si>
+  <si>
+    <t>declaracion de variables</t>
+  </si>
+  <si>
+    <t>inicializacion de variable</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>"0918724530"</t>
+  </si>
+  <si>
+    <t>clase1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gato</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Perro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <t>Gato</t>
+  </si>
+  <si>
+    <t>new Perro()</t>
+  </si>
+  <si>
+    <t>new Gato()</t>
+  </si>
+  <si>
+    <t>Perro</t>
+  </si>
+  <si>
+    <t>clase2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1370,8 +1520,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1417,6 +1596,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1533,7 +1730,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1600,6 +1797,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -4208,8 +4425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F2:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4486,4 +4703,219 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:Y26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="31"/>
+    <col min="2" max="3" width="6.5703125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="12" style="31" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3" style="38" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="31" customWidth="1"/>
+    <col min="8" max="13" width="6.5703125" style="31" customWidth="1"/>
+    <col min="14" max="14" width="3.5703125" style="31" customWidth="1"/>
+    <col min="15" max="15" width="2.7109375" style="41" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="31" customWidth="1"/>
+    <col min="17" max="26" width="4.42578125" style="31" customWidth="1"/>
+    <col min="27" max="16384" width="11.42578125" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:25">
+      <c r="Q1" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="4:25">
+      <c r="D2" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="4:25">
+      <c r="D3" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="R3" s="39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="4:25">
+      <c r="T4" s="40"/>
+    </row>
+    <row r="5" spans="4:25" ht="18.75">
+      <c r="D5" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="T5" s="40"/>
+    </row>
+    <row r="6" spans="4:25">
+      <c r="R6" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+    </row>
+    <row r="7" spans="4:25">
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+    </row>
+    <row r="8" spans="4:25" ht="18.75">
+      <c r="D8" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="G8" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="4:25">
+      <c r="R9" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="40"/>
+    </row>
+    <row r="10" spans="4:25" ht="18.75">
+      <c r="D10" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="U10" s="40"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="40"/>
+    </row>
+    <row r="11" spans="4:25">
+      <c r="U11" s="40"/>
+      <c r="V11" s="40"/>
+      <c r="W11" s="40"/>
+      <c r="X11" s="40"/>
+      <c r="Y11" s="40"/>
+    </row>
+    <row r="12" spans="4:25">
+      <c r="Q12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="U12" s="40"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="40"/>
+      <c r="X12" s="40"/>
+      <c r="Y12" s="40"/>
+    </row>
+    <row r="13" spans="4:25">
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="40"/>
+      <c r="Y13" s="40"/>
+    </row>
+    <row r="14" spans="4:25">
+      <c r="Q14" s="38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="4:25">
+      <c r="R16" s="39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="17:21">
+      <c r="T17" s="40"/>
+    </row>
+    <row r="18" spans="17:21">
+      <c r="T18" s="40"/>
+    </row>
+    <row r="19" spans="17:21">
+      <c r="R19" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+    </row>
+    <row r="20" spans="17:21">
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+    </row>
+    <row r="21" spans="17:21">
+      <c r="R21" s="40"/>
+      <c r="S21" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="17:21">
+      <c r="R22" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="S22" s="40"/>
+    </row>
+    <row r="23" spans="17:21">
+      <c r="U23" s="40"/>
+    </row>
+    <row r="24" spans="17:21">
+      <c r="U24" s="40"/>
+    </row>
+    <row r="25" spans="17:21">
+      <c r="Q25" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="U25" s="40"/>
+    </row>
+    <row r="26" spans="17:21">
+      <c r="U26" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>